<commit_message>
begun documentation of OM
</commit_message>
<xml_diff>
--- a/data-raw/allfile.xlsx
+++ b/data-raw/allfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\A_Code\aMSE\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C6410D8-AC6F-4A61-814D-10393E3F63F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E325684A-D9B4-4E59-8197-D1A3089E94B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
   </bookViews>
   <sheets>
     <sheet name="allfile" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="288">
+  <si>
+    <t>syntax</t>
+  </si>
+  <si>
+    <t>linenumber</t>
+  </si>
   <si>
     <t>file</t>
   </si>
   <si>
-    <t>syntax</t>
-  </si>
-  <si>
-    <t>linenumber</t>
-  </si>
-  <si>
     <t>function</t>
   </si>
   <si>
     <t>references</t>
   </si>
   <si>
+    <t>projection1</t>
+  </si>
+  <si>
+    <t>addrepvar(zoneC,zoneDR,inHt,glb,ctrl,nyrs=25,reset=TRUE)</t>
+  </si>
+  <si>
+    <t>projection</t>
+  </si>
+  <si>
+    <t>addrepvar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getvar, getvect, oneyear, oneyearrec, </t>
+  </si>
+  <si>
+    <t>projection2</t>
+  </si>
+  <si>
+    <t>asSAU(zoneDP,sauindex,saunames,b0,exb0)</t>
+  </si>
+  <si>
+    <t>asSAU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, calcsau, sumpops, </t>
+  </si>
+  <si>
     <t>generate_results1</t>
   </si>
   <si>
@@ -52,6 +79,18 @@
     <t xml:space="preserve">, getlistvar, maturity, </t>
   </si>
   <si>
+    <t>projection3</t>
+  </si>
+  <si>
+    <t>calcsau(invar,saunames,ref0)</t>
+  </si>
+  <si>
+    <t>calcsau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
     <t>generate_results2</t>
   </si>
   <si>
@@ -61,7 +100,19 @@
     <t>compzoneN</t>
   </si>
   <si>
-    <t xml:space="preserve">, </t>
+    <t>HS-HCR1</t>
+  </si>
+  <si>
+    <t>constCatch(inTAC,zoneDP,glob,ctrl,projyrs,inityrs=10)</t>
+  </si>
+  <si>
+    <t>HS-HCR</t>
+  </si>
+  <si>
+    <t>constCatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getvect, oneyear, oneyearcat, oneyearrec, </t>
   </si>
   <si>
     <t>inputfiles1</t>
@@ -112,13 +163,13 @@
     <t>dynamics1</t>
   </si>
   <si>
-    <t>depleteSAU(zoneC,zoneD,glob,depl,product,len=15)</t>
+    <t>depletepop(zoneC,zoneD,glob,depl,product,len=15)</t>
   </si>
   <si>
     <t>dynamics</t>
   </si>
   <si>
-    <t>depleteSAU</t>
+    <t>depletepop</t>
   </si>
   <si>
     <t xml:space="preserve">, runthreeH, </t>
@@ -187,15 +238,12 @@
     <t>findmsy</t>
   </si>
   <si>
-    <t>HS-HCR1</t>
+    <t>HS-HCR2</t>
   </si>
   <si>
     <t>getaav(invect)</t>
   </si>
   <si>
-    <t>HS-HCR</t>
-  </si>
-  <si>
     <t>getaav</t>
   </si>
   <si>
@@ -211,7 +259,7 @@
     <t>getConst</t>
   </si>
   <si>
-    <t>HS-HCR2</t>
+    <t>HS-HCR3</t>
   </si>
   <si>
     <t>getgrad1(vectce)</t>
@@ -220,7 +268,7 @@
     <t>getgrad1</t>
   </si>
   <si>
-    <t>HS-HCR3</t>
+    <t>HS-HCR4</t>
   </si>
   <si>
     <t>getgrad4(vectce,wid=4)</t>
@@ -268,7 +316,7 @@
     <t xml:space="preserve">, getsum, </t>
   </si>
   <si>
-    <t>HS-HCR4</t>
+    <t>HS-HCR5</t>
   </si>
   <si>
     <t>getscore(grad14)</t>
@@ -364,6 +412,18 @@
     <t xml:space="preserve">, getvar, </t>
   </si>
   <si>
+    <t>RcppExports1</t>
+  </si>
+  <si>
+    <t>invC(x)</t>
+  </si>
+  <si>
+    <t>RcppExports</t>
+  </si>
+  <si>
+    <t>invC</t>
+  </si>
+  <si>
     <t>defineZone9</t>
   </si>
   <si>
@@ -433,6 +493,15 @@
     <t xml:space="preserve">, defineBlock, definepops, getvar, makeabpop, makemove, oneyrgrowth, </t>
   </si>
   <si>
+    <t>projection4</t>
+  </si>
+  <si>
+    <t>makezoneDR(projyr,iter,glob,inzoneD)</t>
+  </si>
+  <si>
+    <t>makezoneDR</t>
+  </si>
+  <si>
     <t>defineZone14</t>
   </si>
   <si>
@@ -445,6 +514,18 @@
     <t>defineZone15</t>
   </si>
   <si>
+    <t>modprojC(zoneC,glob,inzone)</t>
+  </si>
+  <si>
+    <t>modprojC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getlistvar, getvar, logistic, </t>
+  </si>
+  <si>
+    <t>defineZone16</t>
+  </si>
+  <si>
     <t>modzoneC(zoneC,zoneD,glob,lowlim=0.0,uplim=0.4,inc=0.005)</t>
   </si>
   <si>
@@ -454,6 +535,24 @@
     <t xml:space="preserve">, doproduction, findmsy, </t>
   </si>
   <si>
+    <t>defineZone17</t>
+  </si>
+  <si>
+    <t>modzoneCSel(zoneC,sel,selwt,glb,yrs)</t>
+  </si>
+  <si>
+    <t>modzoneCSel</t>
+  </si>
+  <si>
+    <t>RcppExports2</t>
+  </si>
+  <si>
+    <t>mvC(inmat,invect)</t>
+  </si>
+  <si>
+    <t>mvC</t>
+  </si>
+  <si>
     <t>generate_results3</t>
   </si>
   <si>
@@ -484,7 +583,7 @@
     <t>dynamics4</t>
   </si>
   <si>
-    <t>oneyearC(zoneC,zoneD,Ncl,catchp,year,sigmar,npop,movem)</t>
+    <t>oneyearC(zoneC,zoneDP,catchp,year,iter,sigmar,Ncl,npop,movem)</t>
   </si>
   <si>
     <t>oneyearC</t>
@@ -505,15 +604,12 @@
     <t>dynamics5</t>
   </si>
   <si>
-    <t>oneyearD(zoneC,zoneD,Ncl,inHt,year,sigmar,npop,movem)</t>
+    <t>oneyearD(zoneC,zoneD,inHt,year,sigmar,Ncl,npop,movem)</t>
   </si>
   <si>
     <t>oneyearD</t>
   </si>
   <si>
-    <t xml:space="preserve">, getvar, getvect, oneyear, oneyearrec, </t>
-  </si>
-  <si>
     <t>dynamics6</t>
   </si>
   <si>
@@ -574,7 +670,7 @@
     <t xml:space="preserve">, findmsy, plotprod, </t>
   </si>
   <si>
-    <t>defineZone17</t>
+    <t>defineZone19</t>
   </si>
   <si>
     <t>print.zone(x,...)</t>
@@ -586,7 +682,7 @@
     <t xml:space="preserve">, getlistvar, </t>
   </si>
   <si>
-    <t>defineZone16</t>
+    <t>defineZone18</t>
   </si>
   <si>
     <t>print.zoneDefinition(x,...)</t>
@@ -649,7 +745,16 @@
     <t>replaceVar</t>
   </si>
   <si>
-    <t>defineZone18</t>
+    <t>defineZone21</t>
+  </si>
+  <si>
+    <t>resetexB0(zoneC,zoneD)</t>
+  </si>
+  <si>
+    <t>resetexB0</t>
+  </si>
+  <si>
+    <t>defineZone20</t>
   </si>
   <si>
     <t>resetLML(inzone,inLML,inyear,glob)</t>
@@ -670,7 +775,7 @@
     <t>resetSel</t>
   </si>
   <si>
-    <t>defineZone19</t>
+    <t>dynamics8</t>
   </si>
   <si>
     <t>restart(oldzoneD,nyrs,npop,N,zero=TRUE)</t>
@@ -679,7 +784,7 @@
     <t>restart</t>
   </si>
   <si>
-    <t>defineZone20</t>
+    <t>dynamics9</t>
   </si>
   <si>
     <t>runthreeH(zoneC,zoneD,inHarv,glob,maxiter=3)</t>
@@ -700,7 +805,7 @@
     <t>scaletoOne</t>
   </si>
   <si>
-    <t>defineZone21</t>
+    <t>defineZone22</t>
   </si>
   <si>
     <t>setupzone(constants,zone1,uplim=0.4,inc=0.005)</t>
@@ -712,7 +817,7 @@
     <t xml:space="preserve">, makezone, makezoneC, modzoneC, </t>
   </si>
   <si>
-    <t>defineZone22</t>
+    <t>defineZone23</t>
   </si>
   <si>
     <t>STM(p,mids)</t>
@@ -733,7 +838,25 @@
     <t>summarizeprod</t>
   </si>
   <si>
-    <t>HS-HCR5</t>
+    <t>projection5</t>
+  </si>
+  <si>
+    <t>sumpops(invar,sauindex,saunames)</t>
+  </si>
+  <si>
+    <t>sumpops</t>
+  </si>
+  <si>
+    <t>RcppExports3</t>
+  </si>
+  <si>
+    <t>svvC(lhs,rhs)</t>
+  </si>
+  <si>
+    <t>svvC</t>
+  </si>
+  <si>
+    <t>HS-HCR6</t>
   </si>
   <si>
     <t>targblockHCR(incpueBlock,targetCE,modifyTarg=1.0)</t>
@@ -742,7 +865,7 @@
     <t>targblockHCR</t>
   </si>
   <si>
-    <t>defineZone23</t>
+    <t>defineZone24</t>
   </si>
   <si>
     <t>testequil(zoneC,zoneD,glb,inH=0.0,verbose=TRUE)</t>
@@ -751,13 +874,16 @@
     <t>testequil</t>
   </si>
   <si>
-    <t>defineZone24</t>
+    <t>defineZone25</t>
   </si>
   <si>
     <t>WtatLen(ina,inb,lens)</t>
   </si>
   <si>
     <t>WtatLen</t>
+  </si>
+  <si>
+    <t>Rfile</t>
   </si>
 </sst>
 </file>
@@ -1581,30 +1707,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1615,599 +1745,599 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C3">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>255</v>
       </c>
       <c r="C5">
-        <v>177</v>
+        <v>498</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>256</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>282</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>1119</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>283</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>261</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>262</v>
       </c>
       <c r="C7">
-        <v>74</v>
+        <v>1018</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>263</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
       <c r="C8">
-        <v>45</v>
+        <v>519</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9">
-        <v>131</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>245</v>
       </c>
       <c r="C10">
-        <v>165</v>
+        <v>953</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>246</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>248</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>249</v>
       </c>
       <c r="C11">
-        <v>230</v>
+        <v>704</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>250</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>290</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>339</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>194</v>
       </c>
       <c r="C14">
-        <v>388</v>
+        <v>327</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>195</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>187</v>
       </c>
       <c r="C15">
-        <v>440</v>
+        <v>257</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>188</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>429</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="C17">
-        <v>18</v>
+        <v>693</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="C18">
-        <v>44</v>
+        <v>227</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>223</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>224</v>
       </c>
       <c r="C19">
-        <v>71</v>
+        <v>343</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>225</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
       <c r="C21">
-        <v>103</v>
+        <v>780</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="C22">
-        <v>130</v>
+        <v>927</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>227</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
       <c r="C23">
-        <v>227</v>
+        <v>396</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>229</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>234</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>235</v>
       </c>
       <c r="C24">
-        <v>104</v>
+        <v>582</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>236</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C25">
         <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>231</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="C26">
-        <v>267</v>
+        <v>545</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>238</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>239</v>
       </c>
       <c r="C27">
-        <v>286</v>
+        <v>667</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>94</v>
+        <v>240</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>213</v>
       </c>
       <c r="C28">
-        <v>326</v>
+        <v>373</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>214</v>
       </c>
       <c r="F28" t="s">
-        <v>13</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>167</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="C29">
-        <v>494</v>
+        <v>831</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="C30">
-        <v>516</v>
+        <v>629</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>11</v>
       </c>
       <c r="C31">
-        <v>164</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
@@ -2215,825 +2345,1068 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>391</v>
+        <v>133</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>429</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>484</v>
+        <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="C35">
-        <v>519</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="C36">
-        <v>283</v>
+        <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E36" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="C37">
-        <v>311</v>
+        <v>131</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="C38">
-        <v>590</v>
+        <v>290</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C39">
-        <v>691</v>
+        <v>339</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="F39" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="C40">
-        <v>627</v>
+        <v>388</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="F40" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="C41">
-        <v>756</v>
+        <v>440</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="C42">
-        <v>792</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="C43">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>78</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C44">
-        <v>217</v>
+        <v>107</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>149</v>
+        <v>81</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>83</v>
       </c>
       <c r="C45">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E45" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
       <c r="F45" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="C46">
-        <v>250</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E46" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
       <c r="F46" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>89</v>
       </c>
       <c r="C47">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
       <c r="C48">
-        <v>320</v>
+        <v>130</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="F48" t="s">
-        <v>163</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C49">
-        <v>372</v>
+        <v>167</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E49" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="F49" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="C50">
-        <v>405</v>
+        <v>267</v>
       </c>
       <c r="D50" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="F50" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="C51">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E51" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="F51" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="C52">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>113</v>
       </c>
       <c r="F52" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="C53">
-        <v>36</v>
+        <v>495</v>
       </c>
       <c r="D53" t="s">
-        <v>178</v>
+        <v>77</v>
       </c>
       <c r="E53" t="s">
-        <v>179</v>
+        <v>116</v>
       </c>
       <c r="F53" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>181</v>
+        <v>118</v>
       </c>
       <c r="C54">
-        <v>373</v>
+        <v>517</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E54" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
       <c r="F54" t="s">
-        <v>183</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="B55" t="s">
-        <v>185</v>
+        <v>121</v>
       </c>
       <c r="C55">
-        <v>856</v>
+        <v>164</v>
       </c>
       <c r="D55" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E55" t="s">
-        <v>186</v>
+        <v>122</v>
       </c>
       <c r="F55" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>189</v>
+        <v>124</v>
       </c>
       <c r="C56">
-        <v>818</v>
+        <v>391</v>
       </c>
       <c r="D56" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
-        <v>190</v>
+        <v>125</v>
       </c>
       <c r="F56" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>191</v>
+        <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>131</v>
       </c>
       <c r="C57">
-        <v>343</v>
+        <v>13</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="E57" t="s">
-        <v>193</v>
+        <v>133</v>
       </c>
       <c r="F57" t="s">
-        <v>194</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>195</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
       <c r="C58">
-        <v>396</v>
+        <v>484</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E58" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="F58" t="s">
-        <v>198</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="B59" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="C59">
-        <v>538</v>
+        <v>283</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E59" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="C60">
-        <v>575</v>
+        <v>311</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E60" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
       <c r="F60" t="s">
-        <v>205</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>206</v>
+        <v>147</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>148</v>
       </c>
       <c r="C61">
-        <v>660</v>
+        <v>592</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E61" t="s">
-        <v>208</v>
+        <v>149</v>
       </c>
       <c r="F61" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="B62" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="C62">
-        <v>882</v>
+        <v>160</v>
       </c>
       <c r="D62" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="F62" t="s">
-        <v>212</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>160</v>
       </c>
       <c r="B63" t="s">
-        <v>214</v>
+        <v>161</v>
       </c>
       <c r="C63">
-        <v>697</v>
+        <v>758</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E63" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
       <c r="F63" t="s">
-        <v>212</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="C64">
-        <v>923</v>
+        <v>863</v>
       </c>
       <c r="D64" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E64" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="F64" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="C65">
-        <v>975</v>
+        <v>28</v>
       </c>
       <c r="D65" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="E65" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="F65" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="B66" t="s">
-        <v>224</v>
+        <v>178</v>
       </c>
       <c r="C66">
-        <v>740</v>
+        <v>160</v>
       </c>
       <c r="D66" t="s">
         <v>16</v>
       </c>
       <c r="E66" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="F66" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>226</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>227</v>
+        <v>181</v>
       </c>
       <c r="C67">
-        <v>1014</v>
+        <v>217</v>
       </c>
       <c r="D67" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E67" t="s">
-        <v>228</v>
+        <v>182</v>
       </c>
       <c r="F67" t="s">
-        <v>229</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>230</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="C68">
-        <v>1061</v>
+        <v>113</v>
       </c>
       <c r="D68" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="F68" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="B69" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="C69">
-        <v>29</v>
+        <v>179</v>
       </c>
       <c r="D69" t="s">
-        <v>235</v>
+        <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="F69" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="B70" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
       <c r="C70">
-        <v>135</v>
+        <v>379</v>
       </c>
       <c r="D70" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E70" t="s">
-        <v>239</v>
+        <v>198</v>
       </c>
       <c r="F70" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="B71" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="C71">
-        <v>1116</v>
+        <v>412</v>
       </c>
       <c r="D71" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E71" t="s">
-        <v>242</v>
+        <v>201</v>
       </c>
       <c r="F71" t="s">
-        <v>222</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>202</v>
+      </c>
+      <c r="B72" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72">
+        <v>276</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" t="s">
+        <v>204</v>
+      </c>
+      <c r="F72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>205</v>
+      </c>
+      <c r="B73" t="s">
+        <v>206</v>
+      </c>
+      <c r="C73">
+        <v>331</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>207</v>
+      </c>
+      <c r="F73" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>208</v>
+      </c>
+      <c r="B74" t="s">
+        <v>209</v>
+      </c>
+      <c r="C74">
+        <v>36</v>
+      </c>
+      <c r="D74" t="s">
+        <v>210</v>
+      </c>
+      <c r="E74" t="s">
+        <v>211</v>
+      </c>
+      <c r="F74" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>220</v>
+      </c>
+      <c r="B75" t="s">
+        <v>221</v>
+      </c>
+      <c r="C75">
+        <v>889</v>
+      </c>
+      <c r="D75" t="s">
+        <v>41</v>
+      </c>
+      <c r="E75" t="s">
+        <v>222</v>
+      </c>
+      <c r="F75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>241</v>
+      </c>
+      <c r="B76" t="s">
+        <v>242</v>
+      </c>
+      <c r="C76">
+        <v>986</v>
+      </c>
+      <c r="D76" t="s">
+        <v>41</v>
+      </c>
+      <c r="E76" t="s">
         <v>243</v>
       </c>
-      <c r="B72" t="s">
-        <v>244</v>
-      </c>
-      <c r="C72">
-        <v>1176</v>
-      </c>
-      <c r="D72" t="s">
-        <v>24</v>
-      </c>
-      <c r="E72" t="s">
-        <v>245</v>
-      </c>
-      <c r="F72" t="s">
-        <v>13</v>
+      <c r="F76" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>251</v>
+      </c>
+      <c r="B77" t="s">
+        <v>252</v>
+      </c>
+      <c r="C77">
+        <v>446</v>
+      </c>
+      <c r="D77" t="s">
+        <v>48</v>
+      </c>
+      <c r="E77" t="s">
+        <v>253</v>
+      </c>
+      <c r="F77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>258</v>
+      </c>
+      <c r="B78" t="s">
+        <v>259</v>
+      </c>
+      <c r="C78">
+        <v>747</v>
+      </c>
+      <c r="D78" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" t="s">
+        <v>260</v>
+      </c>
+      <c r="F78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>265</v>
+      </c>
+      <c r="B79" t="s">
+        <v>266</v>
+      </c>
+      <c r="C79">
+        <v>1064</v>
+      </c>
+      <c r="D79" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79" t="s">
+        <v>267</v>
+      </c>
+      <c r="F79" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>268</v>
+      </c>
+      <c r="B80" t="s">
+        <v>269</v>
+      </c>
+      <c r="C80">
+        <v>29</v>
+      </c>
+      <c r="D80" t="s">
+        <v>270</v>
+      </c>
+      <c r="E80" t="s">
+        <v>271</v>
+      </c>
+      <c r="F80" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>272</v>
+      </c>
+      <c r="B81" t="s">
+        <v>273</v>
+      </c>
+      <c r="C81">
+        <v>211</v>
+      </c>
+      <c r="D81" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" t="s">
+        <v>274</v>
+      </c>
+      <c r="F81" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>275</v>
+      </c>
+      <c r="B82" t="s">
+        <v>276</v>
+      </c>
+      <c r="C82">
+        <v>40</v>
+      </c>
+      <c r="D82" t="s">
+        <v>132</v>
+      </c>
+      <c r="E82" t="s">
+        <v>277</v>
+      </c>
+      <c r="F82" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" t="s">
+        <v>279</v>
+      </c>
+      <c r="C83">
+        <v>198</v>
+      </c>
+      <c r="D83" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" t="s">
+        <v>280</v>
+      </c>
+      <c r="F83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>284</v>
+      </c>
+      <c r="B84" t="s">
+        <v>285</v>
+      </c>
+      <c r="C84">
+        <v>1179</v>
+      </c>
+      <c r="D84" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" t="s">
+        <v>286</v>
+      </c>
+      <c r="F84" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F84">
+    <sortCondition descending="1" ref="F2:F84"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Starting to make the dynamics consistent between conditioning and projections. More to do.
</commit_message>
<xml_diff>
--- a/data-raw/allfile.xlsx
+++ b/data-raw/allfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\A_Code\aMSE\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E325684A-D9B4-4E59-8197-D1A3089E94B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40A0DF-D77C-46AE-8D4F-AD6059FDF556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allfile" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="317">
   <si>
     <t>syntax</t>
   </si>
@@ -40,13 +40,13 @@
     <t>projection1</t>
   </si>
   <si>
-    <t>addrepvar(zoneC,zoneDR,inHt,glb,ctrl,nyrs=25,reset=TRUE)</t>
+    <t>addrecvar(zoneC,zoneDR,inHt,glb,ctrl,aspcatch,nyrs=25,reset=TRUE)</t>
   </si>
   <si>
     <t>projection</t>
   </si>
   <si>
-    <t>addrepvar</t>
+    <t>addrecvar</t>
   </si>
   <si>
     <t xml:space="preserve">, getvar, getvect, oneyear, oneyearrec, </t>
@@ -55,7 +55,7 @@
     <t>projection2</t>
   </si>
   <si>
-    <t>asSAU(zoneDP,sauindex,saunames,b0,exb0)</t>
+    <t>asSAU(projzone,sauindex,saunames,b0,exb0)</t>
   </si>
   <si>
     <t>asSAU</t>
@@ -64,6 +64,18 @@
     <t xml:space="preserve">, calcsau, sumpops, </t>
   </si>
   <si>
+    <t>projection3</t>
+  </si>
+  <si>
+    <t>aszone(sauzone,zoneCP)</t>
+  </si>
+  <si>
+    <t>aszone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getvar, </t>
+  </si>
+  <si>
     <t>generate_results1</t>
   </si>
   <si>
@@ -79,7 +91,19 @@
     <t xml:space="preserve">, getlistvar, maturity, </t>
   </si>
   <si>
-    <t>projection3</t>
+    <t>projection4</t>
+  </si>
+  <si>
+    <t>calcprojsel(zoneC,projC,glb)</t>
+  </si>
+  <si>
+    <t>calcprojsel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, logistic, </t>
+  </si>
+  <si>
+    <t>projection5</t>
   </si>
   <si>
     <t>calcsau(invar,saunames,ref0)</t>
@@ -103,7 +127,7 @@
     <t>HS-HCR1</t>
   </si>
   <si>
-    <t>constCatch(inTAC,zoneDP,glob,ctrl,projyrs,inityrs=10)</t>
+    <t>constCatch(inTAC,zoneCP,zoneDP,glob,ctrl,projyrs,inityrs=10)</t>
   </si>
   <si>
     <t>HS-HCR</t>
@@ -163,13 +187,13 @@
     <t>dynamics1</t>
   </si>
   <si>
-    <t>depletepop(zoneC,zoneD,glob,depl,product,len=15)</t>
+    <t>depleteSAU(zoneC,zoneD,glob,initdepl,product,len=15)</t>
   </si>
   <si>
     <t>dynamics</t>
   </si>
   <si>
-    <t>depletepop</t>
+    <t>depleteSAU</t>
   </si>
   <si>
     <t xml:space="preserve">, runthreeH, </t>
@@ -193,6 +217,18 @@
     <t>dodepletion</t>
   </si>
   <si>
+    <t>dynamics2</t>
+  </si>
+  <si>
+    <t>dohistoricC(zoneDD,zoneC,glob,condC,sigR=1e-08)</t>
+  </si>
+  <si>
+    <t>dohistoricC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, oneyear, oneyearsauC, </t>
+  </si>
+  <si>
     <t>defineZone4</t>
   </si>
   <si>
@@ -202,6 +238,15 @@
     <t>doproduction</t>
   </si>
   <si>
+    <t>projection6</t>
+  </si>
+  <si>
+    <t>doprojection(zoneCP,zoneDP,glob,ctrl,projyrs,applyHS,hsargs,</t>
+  </si>
+  <si>
+    <t>doprojection</t>
+  </si>
+  <si>
     <t>defineZone5</t>
   </si>
   <si>
@@ -259,24 +304,6 @@
     <t>getConst</t>
   </si>
   <si>
-    <t>HS-HCR3</t>
-  </si>
-  <si>
-    <t>getgrad1(vectce)</t>
-  </si>
-  <si>
-    <t>getgrad1</t>
-  </si>
-  <si>
-    <t>HS-HCR4</t>
-  </si>
-  <si>
-    <t>getgrad4(vectce,wid=4)</t>
-  </si>
-  <si>
-    <t>getgrad4</t>
-  </si>
-  <si>
     <t>getfunctions2</t>
   </si>
   <si>
@@ -307,7 +334,7 @@
     <t>getfunctions7</t>
   </si>
   <si>
-    <t>getsauzone(zoneD)</t>
+    <t>getsauzone(zoneD,glb)</t>
   </si>
   <si>
     <t>getsauzone</t>
@@ -316,15 +343,6 @@
     <t xml:space="preserve">, getsum, </t>
   </si>
   <si>
-    <t>HS-HCR5</t>
-  </si>
-  <si>
-    <t>getscore(grad14)</t>
-  </si>
-  <si>
-    <t>getscore</t>
-  </si>
-  <si>
     <t>getfunctions6</t>
   </si>
   <si>
@@ -409,9 +427,6 @@
     <t>getzoneprops</t>
   </si>
   <si>
-    <t xml:space="preserve">, getvar, </t>
-  </si>
-  <si>
     <t>RcppExports1</t>
   </si>
   <si>
@@ -445,6 +460,18 @@
     <t xml:space="preserve">, logistic, maturity, STM, WtatLen, </t>
   </si>
   <si>
+    <t>defineZone11</t>
+  </si>
+  <si>
+    <t>makeequilzone(resdir,ctrlfile="control.csv",cleanslate=FALSE)</t>
+  </si>
+  <si>
+    <t>makeequilzone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, readctrlfile, readdatafile, resetexB0, setupzone, testequil, </t>
+  </si>
+  <si>
     <t>inputfiles4</t>
   </si>
   <si>
@@ -463,7 +490,7 @@
     <t>makeLabel</t>
   </si>
   <si>
-    <t>defineZone11</t>
+    <t>defineZone12</t>
   </si>
   <si>
     <t>makemove(npop,recs,ld,sigmove=0.0)</t>
@@ -472,18 +499,18 @@
     <t>makemove</t>
   </si>
   <si>
+    <t>defineZone14</t>
+  </si>
+  <si>
+    <t>makezone(glob,zoneC)</t>
+  </si>
+  <si>
+    <t>makezone</t>
+  </si>
+  <si>
     <t>defineZone13</t>
   </si>
   <si>
-    <t>makezone(glob,zoneC)</t>
-  </si>
-  <si>
-    <t>makezone</t>
-  </si>
-  <si>
-    <t>defineZone12</t>
-  </si>
-  <si>
     <t>makezoneC(zone,const)</t>
   </si>
   <si>
@@ -493,16 +520,25 @@
     <t xml:space="preserve">, defineBlock, definepops, getvar, makeabpop, makemove, oneyrgrowth, </t>
   </si>
   <si>
-    <t>projection4</t>
-  </si>
-  <si>
-    <t>makezoneDR(projyr,iter,glob,inzoneD)</t>
+    <t>projection7</t>
+  </si>
+  <si>
+    <t>makezoneDP(projyr,iter,glb,inzoneD)</t>
+  </si>
+  <si>
+    <t>makezoneDP</t>
+  </si>
+  <si>
+    <t>projection8</t>
+  </si>
+  <si>
+    <t>makezoneDR(projyr,iter,glb,inzoneD)</t>
   </si>
   <si>
     <t>makezoneDR</t>
   </si>
   <si>
-    <t>defineZone14</t>
+    <t>defineZone15</t>
   </si>
   <si>
     <t>maturity(ina,inb,lens)</t>
@@ -511,10 +547,10 @@
     <t>maturity</t>
   </si>
   <si>
-    <t>defineZone15</t>
-  </si>
-  <si>
-    <t>modprojC(zoneC,glob,inzone)</t>
+    <t>projection9</t>
+  </si>
+  <si>
+    <t>modprojC(zoneC,glob,projC)</t>
   </si>
   <si>
     <t>modprojC</t>
@@ -535,361 +571,412 @@
     <t xml:space="preserve">, doproduction, findmsy, </t>
   </si>
   <si>
+    <t>projection10</t>
+  </si>
+  <si>
+    <t>modzoneCSel(zoneC,sel,selwt,glb,yrs)</t>
+  </si>
+  <si>
+    <t>modzoneCSel</t>
+  </si>
+  <si>
+    <t>RcppExports2</t>
+  </si>
+  <si>
+    <t>mvC(inmat,invect)</t>
+  </si>
+  <si>
+    <t>mvC</t>
+  </si>
+  <si>
+    <t>generate_results3</t>
+  </si>
+  <si>
+    <t>numbersatsize(resdir,glb,zoneD)</t>
+  </si>
+  <si>
+    <t>numbersatsize</t>
+  </si>
+  <si>
+    <t>generate_results4</t>
+  </si>
+  <si>
+    <t>numbersatsizeSAU(resdir,glb,zoneC,zoneD,sau,yr=1,</t>
+  </si>
+  <si>
+    <t>numbersatsizeSAU</t>
+  </si>
+  <si>
+    <t>dynamics3</t>
+  </si>
+  <si>
+    <t>oneyear(inpopC,inNt,Nclass,inH,yr)</t>
+  </si>
+  <si>
+    <t>oneyear</t>
+  </si>
+  <si>
+    <t>dynamics6</t>
+  </si>
+  <si>
+    <t>oneyearC(zoneC,zoneDP,catchp,year,iter,sigmar,Ncl,npop,movem)</t>
+  </si>
+  <si>
+    <t>oneyearC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getvar, getvect, oneyear, oneyearcat, oneyearrec, </t>
+  </si>
+  <si>
+    <t>dynamics4</t>
+  </si>
+  <si>
+    <t>oneyearcat(inpopC,inNt,Nclass,incat,yr)</t>
+  </si>
+  <si>
+    <t>oneyearcat</t>
+  </si>
+  <si>
+    <t>dynamics7</t>
+  </si>
+  <si>
+    <t>oneyearD(zoneC,zoneD,inHt,year,sigmar,Ncl,npop,movem)</t>
+  </si>
+  <si>
+    <t>oneyearD</t>
+  </si>
+  <si>
+    <t>dynamics8</t>
+  </si>
+  <si>
+    <t>oneyearrec(steep,R0,B0,Bsp,sigR)</t>
+  </si>
+  <si>
+    <t>oneyearrec</t>
+  </si>
+  <si>
+    <t>dynamics5</t>
+  </si>
+  <si>
+    <t>oneyearsauC(zoneC,zoneDD,catchsau,year,sigmar,Ncl,sauindex,movem)</t>
+  </si>
+  <si>
+    <t>oneyearsauC</t>
+  </si>
+  <si>
+    <t>dynamics9</t>
+  </si>
+  <si>
+    <t>oneyrgrowth(inpop,startsize=2)</t>
+  </si>
+  <si>
+    <t>oneyrgrowth</t>
+  </si>
+  <si>
+    <t>generate_results5</t>
+  </si>
+  <si>
+    <t>plothistcatch(zone1,pops=NULL,resdir="",defpar=TRUE)</t>
+  </si>
+  <si>
+    <t>plothistcatch</t>
+  </si>
+  <si>
+    <t>generate_results6</t>
+  </si>
+  <si>
+    <t>plothistCE(zone1,pops=NULL,resdir="")</t>
+  </si>
+  <si>
+    <t>plothistCE</t>
+  </si>
+  <si>
+    <t>plotfuns1</t>
+  </si>
+  <si>
+    <t>plotprod(product,xname="MatB",yname="Catch",xlimit=NA,</t>
+  </si>
+  <si>
+    <t>plotfuns</t>
+  </si>
+  <si>
+    <t>plotprod</t>
+  </si>
+  <si>
+    <t>generate_results7</t>
+  </si>
+  <si>
+    <t>plotproductivity(resdir,product,glb)</t>
+  </si>
+  <si>
+    <t>plotproductivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, findmsy, plotprod, </t>
+  </si>
+  <si>
+    <t>plotfuns2</t>
+  </si>
+  <si>
+    <t>plotproj(invar,varlabel,plotconst,miny=0,</t>
+  </si>
+  <si>
+    <t>plotproj</t>
+  </si>
+  <si>
+    <t>plotfuns3</t>
+  </si>
+  <si>
+    <t>plotzoneproj(zoneV,reps,yrs,label="",addqnts=TRUE,miny=0)</t>
+  </si>
+  <si>
+    <t>plotzoneproj</t>
+  </si>
+  <si>
+    <t>projection11</t>
+  </si>
+  <si>
+    <t>poptosau(catvect,cpuevect,sauindex)</t>
+  </si>
+  <si>
+    <t>poptosau</t>
+  </si>
+  <si>
+    <t>projection12</t>
+  </si>
+  <si>
+    <t>prepareprojection(zone1,zoneC,glb,zoneDep,aspcatch)</t>
+  </si>
+  <si>
+    <t>prepareprojection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, addrecvar, makezone, makezoneDR, modprojC, modzoneC, modzoneCSel, </t>
+  </si>
+  <si>
+    <t>defineZone18</t>
+  </si>
+  <si>
+    <t>print.zone(x,...)</t>
+  </si>
+  <si>
+    <t>print.zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getlistvar, </t>
+  </si>
+  <si>
     <t>defineZone17</t>
   </si>
   <si>
-    <t>modzoneCSel(zoneC,sel,selwt,glb,yrs)</t>
-  </si>
-  <si>
-    <t>modzoneCSel</t>
-  </si>
-  <si>
-    <t>RcppExports2</t>
-  </si>
-  <si>
-    <t>mvC(inmat,invect)</t>
-  </si>
-  <si>
-    <t>mvC</t>
-  </si>
-  <si>
-    <t>generate_results3</t>
-  </si>
-  <si>
-    <t>numbersatsize(resdir,glb,zoneD)</t>
-  </si>
-  <si>
-    <t>numbersatsize</t>
-  </si>
-  <si>
-    <t>generate_results4</t>
-  </si>
-  <si>
-    <t>numbersatsizeSAU(resdir,glb,zoneC,zoneD,sau,yr=1,</t>
-  </si>
-  <si>
-    <t>numbersatsizeSAU</t>
-  </si>
-  <si>
-    <t>dynamics2</t>
-  </si>
-  <si>
-    <t>oneyear(inpopC,inNt,Nclass,inH,yr)</t>
-  </si>
-  <si>
-    <t>oneyear</t>
-  </si>
-  <si>
-    <t>dynamics4</t>
-  </si>
-  <si>
-    <t>oneyearC(zoneC,zoneDP,catchp,year,iter,sigmar,Ncl,npop,movem)</t>
-  </si>
-  <si>
-    <t>oneyearC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, getvar, getvect, oneyear, oneyearcat, oneyearrec, </t>
-  </si>
-  <si>
-    <t>dynamics3</t>
-  </si>
-  <si>
-    <t>oneyearcat(inpopC,inNt,Nclass,incat,yr)</t>
-  </si>
-  <si>
-    <t>oneyearcat</t>
-  </si>
-  <si>
-    <t>dynamics5</t>
-  </si>
-  <si>
-    <t>oneyearD(zoneC,zoneD,inHt,year,sigmar,Ncl,npop,movem)</t>
-  </si>
-  <si>
-    <t>oneyearD</t>
-  </si>
-  <si>
-    <t>dynamics6</t>
-  </si>
-  <si>
-    <t>oneyearrec(steep,R0,B0,Bsp,sigR)</t>
-  </si>
-  <si>
-    <t>oneyearrec</t>
-  </si>
-  <si>
-    <t>dynamics7</t>
-  </si>
-  <si>
-    <t>oneyrgrowth(inpop,startsize=2)</t>
-  </si>
-  <si>
-    <t>oneyrgrowth</t>
-  </si>
-  <si>
-    <t>generate_results5</t>
-  </si>
-  <si>
-    <t>plothistcatch(zone1,pops=NULL,resdir="",defpar=TRUE)</t>
-  </si>
-  <si>
-    <t>plothistcatch</t>
-  </si>
-  <si>
-    <t>generate_results6</t>
-  </si>
-  <si>
-    <t>plothistCE(zone1,pops=NULL,resdir="")</t>
-  </si>
-  <si>
-    <t>plothistCE</t>
-  </si>
-  <si>
-    <t>plotfuns1</t>
-  </si>
-  <si>
-    <t>plotprod(product,xname="MatB",yname="Catch",xlimit=NA,</t>
-  </si>
-  <si>
-    <t>plotfuns</t>
-  </si>
-  <si>
-    <t>plotprod</t>
-  </si>
-  <si>
-    <t>generate_results7</t>
-  </si>
-  <si>
-    <t>plotproductivity(resdir,product,glb)</t>
-  </si>
-  <si>
-    <t>plotproductivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, findmsy, plotprod, </t>
+    <t>print.zoneDefinition(x,...)</t>
+  </si>
+  <si>
+    <t>print.zoneDefinition</t>
+  </si>
+  <si>
+    <t>inputfiles6</t>
+  </si>
+  <si>
+    <t>read_conddata(filename)</t>
+  </si>
+  <si>
+    <t>read_conddata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getsingleNum, </t>
+  </si>
+  <si>
+    <t>inputfiles7</t>
+  </si>
+  <si>
+    <t>readctrlfile(datadir,infile="control.csv")</t>
+  </si>
+  <si>
+    <t>readctrlfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getConst, getsingleNum, getStr, </t>
+  </si>
+  <si>
+    <t>inputfiles8</t>
+  </si>
+  <si>
+    <t>readdatafile(numpop,indir,infile)</t>
+  </si>
+  <si>
+    <t>readdatafile</t>
+  </si>
+  <si>
+    <t>inputfiles9</t>
+  </si>
+  <si>
+    <t>readhcrfile(infile)</t>
+  </si>
+  <si>
+    <t>readhcrfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, getConst, getLogical, getsingleNum, getStr, </t>
+  </si>
+  <si>
+    <t>inputfiles10</t>
+  </si>
+  <si>
+    <t>replaceVar(infile,invar,newval)</t>
+  </si>
+  <si>
+    <t>replaceVar</t>
+  </si>
+  <si>
+    <t>defineZone20</t>
+  </si>
+  <si>
+    <t>resetexB0(zoneC,zoneD)</t>
+  </si>
+  <si>
+    <t>resetexB0</t>
   </si>
   <si>
     <t>defineZone19</t>
   </si>
   <si>
-    <t>print.zone(x,...)</t>
-  </si>
-  <si>
-    <t>print.zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, getlistvar, </t>
-  </si>
-  <si>
-    <t>defineZone18</t>
-  </si>
-  <si>
-    <t>print.zoneDefinition(x,...)</t>
-  </si>
-  <si>
-    <t>print.zoneDefinition</t>
-  </si>
-  <si>
-    <t>inputfiles6</t>
-  </si>
-  <si>
-    <t>read_conddata(filename)</t>
-  </si>
-  <si>
-    <t>read_conddata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, getsingleNum, </t>
-  </si>
-  <si>
-    <t>inputfiles7</t>
-  </si>
-  <si>
-    <t>readctrlzone(datadir,infile="control.csv")</t>
-  </si>
-  <si>
-    <t>readctrlzone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, getConst, getsingleNum, getStr, </t>
-  </si>
-  <si>
-    <t>inputfiles8</t>
-  </si>
-  <si>
-    <t>readdatafile(numpop,indir,infile)</t>
-  </si>
-  <si>
-    <t>readdatafile</t>
-  </si>
-  <si>
-    <t>inputfiles9</t>
-  </si>
-  <si>
-    <t>readhcrfile(infile)</t>
-  </si>
-  <si>
-    <t>readhcrfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, getConst, getLogical, getsingleNum, getStr, </t>
-  </si>
-  <si>
-    <t>inputfiles10</t>
-  </si>
-  <si>
-    <t>replaceVar(infile,invar,newval)</t>
-  </si>
-  <si>
-    <t>replaceVar</t>
+    <t>resetLML(inzone,inLML,inyear,glob)</t>
+  </si>
+  <si>
+    <t>resetLML</t>
+  </si>
+  <si>
+    <t>inputfiles11</t>
+  </si>
+  <si>
+    <t>resetSel(inzone,inLML,glob)</t>
+  </si>
+  <si>
+    <t>resetSel</t>
+  </si>
+  <si>
+    <t>dynamics10</t>
+  </si>
+  <si>
+    <t>restart(oldzoneD,nyrs,npop,N,zero=TRUE)</t>
+  </si>
+  <si>
+    <t>restart</t>
+  </si>
+  <si>
+    <t>dynamics11</t>
+  </si>
+  <si>
+    <t>runthreeH(zoneC,zoneD,inHarv,glob,maxiter=3)</t>
+  </si>
+  <si>
+    <t>runthreeH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, oneyear, oneyearD, restart, </t>
+  </si>
+  <si>
+    <t>projection13</t>
+  </si>
+  <si>
+    <t>scaleto1(invect)</t>
+  </si>
+  <si>
+    <t>scaleto1</t>
+  </si>
+  <si>
+    <t>inputfiles12</t>
+  </si>
+  <si>
+    <t>scaletoOne(invect)</t>
+  </si>
+  <si>
+    <t>scaletoOne</t>
   </si>
   <si>
     <t>defineZone21</t>
   </si>
   <si>
-    <t>resetexB0(zoneC,zoneD)</t>
-  </si>
-  <si>
-    <t>resetexB0</t>
-  </si>
-  <si>
-    <t>defineZone20</t>
-  </si>
-  <si>
-    <t>resetLML(inzone,inLML,inyear,glob)</t>
-  </si>
-  <si>
-    <t>resetLML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, logistic, </t>
-  </si>
-  <si>
-    <t>inputfiles11</t>
-  </si>
-  <si>
-    <t>resetSel(inzone,inLML,glob)</t>
-  </si>
-  <si>
-    <t>resetSel</t>
-  </si>
-  <si>
-    <t>dynamics8</t>
-  </si>
-  <si>
-    <t>restart(oldzoneD,nyrs,npop,N,zero=TRUE)</t>
-  </si>
-  <si>
-    <t>restart</t>
-  </si>
-  <si>
-    <t>dynamics9</t>
-  </si>
-  <si>
-    <t>runthreeH(zoneC,zoneD,inHarv,glob,maxiter=3)</t>
-  </si>
-  <si>
-    <t>runthreeH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, oneyear, oneyearD, restart, </t>
-  </si>
-  <si>
-    <t>inputfiles12</t>
-  </si>
-  <si>
-    <t>scaletoOne(invect)</t>
-  </si>
-  <si>
-    <t>scaletoOne</t>
+    <t>setupzone(constants,zone1,uplim=0.4,inc=0.005)</t>
+  </si>
+  <si>
+    <t>setupzone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, makezone, makezoneC, modzoneC, </t>
   </si>
   <si>
     <t>defineZone22</t>
   </si>
   <si>
-    <t>setupzone(constants,zone1,uplim=0.4,inc=0.005)</t>
-  </si>
-  <si>
-    <t>setupzone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">, makezone, makezoneC, modzoneC, </t>
+    <t>STM(p,mids)</t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t>aMSE_utils1</t>
+  </si>
+  <si>
+    <t>summarizeprod(product,saunames)</t>
+  </si>
+  <si>
+    <t>aMSE_utils</t>
+  </si>
+  <si>
+    <t>summarizeprod</t>
+  </si>
+  <si>
+    <t>projection14</t>
+  </si>
+  <si>
+    <t>sumpops(invar,sauindex,saunames)</t>
+  </si>
+  <si>
+    <t>sumpops</t>
+  </si>
+  <si>
+    <t>RcppExports3</t>
+  </si>
+  <si>
+    <t>svvC(lhs,rhs)</t>
+  </si>
+  <si>
+    <t>svvC</t>
   </si>
   <si>
     <t>defineZone23</t>
   </si>
   <si>
-    <t>STM(p,mids)</t>
-  </si>
-  <si>
-    <t>STM</t>
-  </si>
-  <si>
-    <t>aMSE_utils1</t>
-  </si>
-  <si>
-    <t>summarizeprod(product,saunames)</t>
-  </si>
-  <si>
-    <t>aMSE_utils</t>
-  </si>
-  <si>
-    <t>summarizeprod</t>
-  </si>
-  <si>
-    <t>projection5</t>
-  </si>
-  <si>
-    <t>sumpops(invar,sauindex,saunames)</t>
-  </si>
-  <si>
-    <t>sumpops</t>
-  </si>
-  <si>
-    <t>RcppExports3</t>
-  </si>
-  <si>
-    <t>svvC(lhs,rhs)</t>
-  </si>
-  <si>
-    <t>svvC</t>
-  </si>
-  <si>
-    <t>HS-HCR6</t>
-  </si>
-  <si>
-    <t>targblockHCR(incpueBlock,targetCE,modifyTarg=1.0)</t>
-  </si>
-  <si>
-    <t>targblockHCR</t>
+    <t>testequil(zoneC,zoneD,glb,inH=0.0,verbose=TRUE)</t>
+  </si>
+  <si>
+    <t>testequil</t>
   </si>
   <si>
     <t>defineZone24</t>
   </si>
   <si>
-    <t>testequil(zoneC,zoneD,glb,inH=0.0,verbose=TRUE)</t>
-  </si>
-  <si>
-    <t>testequil</t>
-  </si>
-  <si>
-    <t>defineZone25</t>
-  </si>
-  <si>
     <t>WtatLen(ina,inb,lens)</t>
   </si>
   <si>
     <t>WtatLen</t>
   </si>
   <si>
-    <t>Rfile</t>
+    <t>aMSE_utils2</t>
+  </si>
+  <si>
+    <t>wtedmean(x,wts)</t>
+  </si>
+  <si>
+    <t>wtedmean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1706,27 +1793,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>287</v>
-      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1745,156 +1827,156 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>230</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>498</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>257</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>281</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>24</v>
       </c>
       <c r="C6">
-        <v>1119</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>283</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>257</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>1018</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>264</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>519</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
-      </c>
-      <c r="C9">
-        <v>177</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>
@@ -1905,59 +1987,59 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>953</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>246</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>247</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>704</v>
+        <v>279</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
         <v>30</v>
@@ -1965,1448 +2047,1625 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C13">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>55</v>
       </c>
       <c r="C14">
-        <v>327</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>195</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>60</v>
       </c>
       <c r="C15">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="C16">
-        <v>429</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="C17">
-        <v>693</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C18">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>224</v>
+        <v>73</v>
       </c>
       <c r="C19">
-        <v>343</v>
+        <v>253</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C20">
-        <v>21</v>
+        <v>289</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>79</v>
       </c>
       <c r="C21">
-        <v>780</v>
+        <v>338</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>82</v>
       </c>
       <c r="C22">
-        <v>927</v>
+        <v>390</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>218</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s">
-        <v>219</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>227</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>85</v>
       </c>
       <c r="C23">
-        <v>396</v>
+        <v>442</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>229</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>230</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
-        <v>235</v>
+        <v>88</v>
       </c>
       <c r="C24">
-        <v>582</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>236</v>
+        <v>89</v>
       </c>
       <c r="F24" t="s">
-        <v>237</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C25">
-        <v>201</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
       <c r="C26">
-        <v>545</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>233</v>
+        <v>96</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>238</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>239</v>
+        <v>98</v>
       </c>
       <c r="C27">
-        <v>667</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>240</v>
+        <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>101</v>
       </c>
       <c r="C28">
-        <v>373</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>214</v>
+        <v>102</v>
       </c>
       <c r="F28" t="s">
-        <v>215</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="C29">
-        <v>831</v>
+        <v>222</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="C30">
-        <v>629</v>
+        <v>195</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="F30" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C31">
-        <v>97</v>
+        <v>262</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="C32">
-        <v>133</v>
+        <v>282</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="C33">
-        <v>128</v>
+        <v>315</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="C34">
-        <v>27</v>
+        <v>483</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C35">
-        <v>25</v>
+        <v>508</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="E35" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="C36">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="C37">
+        <v>380</v>
+      </c>
+      <c r="D37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" t="s">
         <v>131</v>
       </c>
-      <c r="D37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" t="s">
-        <v>53</v>
-      </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="C38">
-        <v>290</v>
+        <v>415</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="C39">
-        <v>339</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="F39" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
       <c r="C40">
-        <v>388</v>
+        <v>486</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="C41">
-        <v>440</v>
+        <v>521</v>
       </c>
       <c r="D41" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="C42">
-        <v>81</v>
+        <v>585</v>
       </c>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>151</v>
       </c>
       <c r="C43">
-        <v>18</v>
+        <v>385</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
       <c r="C44">
-        <v>107</v>
+        <v>413</v>
       </c>
       <c r="D44" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="C45">
-        <v>134</v>
+        <v>634</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="C46">
-        <v>58</v>
+        <v>736</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E46" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="F46" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="C47">
-        <v>103</v>
+        <v>671</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E47" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>166</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>167</v>
       </c>
       <c r="C48">
-        <v>130</v>
+        <v>347</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>93</v>
+        <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="C49">
-        <v>167</v>
+        <v>409</v>
       </c>
       <c r="D49" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>100</v>
+        <v>171</v>
       </c>
       <c r="F49" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="C50">
-        <v>267</v>
+        <v>802</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="F50" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="C51">
-        <v>286</v>
+        <v>472</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="F51" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>179</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="C52">
-        <v>326</v>
+        <v>840</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="E52" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="F52" t="s">
-        <v>22</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>183</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>184</v>
       </c>
       <c r="C53">
-        <v>495</v>
+        <v>510</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>116</v>
+        <v>185</v>
       </c>
       <c r="F53" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>186</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>187</v>
       </c>
       <c r="C54">
-        <v>517</v>
+        <v>28</v>
       </c>
       <c r="D54" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="E54" t="s">
-        <v>119</v>
+        <v>188</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="C55">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>122</v>
+        <v>191</v>
       </c>
       <c r="F55" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="C56">
-        <v>391</v>
+        <v>217</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>125</v>
+        <v>194</v>
       </c>
       <c r="F56" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>196</v>
       </c>
       <c r="C57">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>197</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>198</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>199</v>
       </c>
       <c r="C58">
-        <v>484</v>
+        <v>360</v>
       </c>
       <c r="D58" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E58" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="C59">
-        <v>283</v>
+        <v>208</v>
       </c>
       <c r="D59" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E59" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="F59" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>144</v>
+        <v>205</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>206</v>
       </c>
       <c r="C60">
-        <v>311</v>
+        <v>426</v>
       </c>
       <c r="D60" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E60" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="F60" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>208</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
+        <v>209</v>
       </c>
       <c r="C61">
-        <v>592</v>
+        <v>477</v>
       </c>
       <c r="D61" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E61" t="s">
-        <v>149</v>
+        <v>210</v>
       </c>
       <c r="F61" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
       <c r="B62" t="s">
-        <v>158</v>
+        <v>212</v>
       </c>
       <c r="C62">
-        <v>160</v>
+        <v>282</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E62" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="F62" t="s">
-        <v>22</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>215</v>
       </c>
       <c r="C63">
-        <v>758</v>
+        <v>510</v>
       </c>
       <c r="D63" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E63" t="s">
-        <v>162</v>
+        <v>216</v>
       </c>
       <c r="F63" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="B64" t="s">
-        <v>172</v>
+        <v>218</v>
       </c>
       <c r="C64">
-        <v>863</v>
+        <v>276</v>
       </c>
       <c r="D64" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="E64" t="s">
-        <v>173</v>
+        <v>219</v>
       </c>
       <c r="F64" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>220</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="C65">
-        <v>28</v>
+        <v>331</v>
       </c>
       <c r="D65" t="s">
-        <v>132</v>
+        <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>176</v>
+        <v>222</v>
       </c>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="B66" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="C66">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>225</v>
       </c>
       <c r="E66" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="F66" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>180</v>
+        <v>227</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="C67">
-        <v>217</v>
+        <v>373</v>
       </c>
       <c r="D67" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E67" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="F67" t="s">
-        <v>22</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>231</v>
       </c>
       <c r="B68" t="s">
-        <v>184</v>
+        <v>232</v>
       </c>
       <c r="C68">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="D68" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="E68" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
       <c r="F68" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="B69" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="C69">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="D69" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="E69" t="s">
-        <v>192</v>
+        <v>236</v>
       </c>
       <c r="F69" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>237</v>
       </c>
       <c r="B70" t="s">
-        <v>197</v>
+        <v>238</v>
       </c>
       <c r="C70">
-        <v>379</v>
+        <v>537</v>
       </c>
       <c r="D70" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>198</v>
+        <v>239</v>
       </c>
       <c r="F70" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>241</v>
       </c>
       <c r="C71">
-        <v>412</v>
+        <v>568</v>
       </c>
       <c r="D71" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>201</v>
+        <v>242</v>
       </c>
       <c r="F71" t="s">
-        <v>22</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="B72" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="C72">
-        <v>276</v>
+        <v>905</v>
       </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E72" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="B73" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="C73">
-        <v>331</v>
+        <v>867</v>
       </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E73" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="F73" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
       <c r="C74">
-        <v>36</v>
+        <v>445</v>
       </c>
       <c r="D74" t="s">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="E74" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="F74" t="s">
-        <v>22</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="B75" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="C75">
-        <v>889</v>
+        <v>501</v>
       </c>
       <c r="D75" t="s">
         <v>41</v>
       </c>
       <c r="E75" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="F75" t="s">
-        <v>22</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="B76" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="C76">
-        <v>986</v>
+        <v>671</v>
       </c>
       <c r="D76" t="s">
         <v>41</v>
       </c>
       <c r="E76" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="F76" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="B77" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="C77">
-        <v>446</v>
+        <v>708</v>
       </c>
       <c r="D77" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E77" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="F77" t="s">
-        <v>22</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B78" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="C78">
-        <v>747</v>
+        <v>793</v>
       </c>
       <c r="D78" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E78" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="F78" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B79" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C79">
-        <v>1064</v>
+        <v>964</v>
       </c>
       <c r="D79" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E79" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="F79" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B80" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C80">
-        <v>29</v>
+        <v>931</v>
       </c>
       <c r="D80" t="s">
-        <v>270</v>
+        <v>49</v>
       </c>
       <c r="E80" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F80" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B81" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C81">
-        <v>211</v>
+        <v>830</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="E81" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F81" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B82" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C82">
-        <v>40</v>
+        <v>544</v>
       </c>
       <c r="D82" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="E82" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B83" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C83">
-        <v>198</v>
+        <v>597</v>
       </c>
       <c r="D83" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E83" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F83" t="s">
-        <v>22</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>285</v>
+      </c>
+      <c r="B84" t="s">
+        <v>286</v>
+      </c>
+      <c r="C84">
+        <v>597</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" t="s">
+        <v>287</v>
+      </c>
+      <c r="F84" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>288</v>
+      </c>
+      <c r="B85" t="s">
+        <v>289</v>
+      </c>
+      <c r="C85">
+        <v>873</v>
+      </c>
+      <c r="D85" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" t="s">
+        <v>290</v>
+      </c>
+      <c r="F85" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>291</v>
+      </c>
+      <c r="B86" t="s">
+        <v>292</v>
+      </c>
+      <c r="C86">
+        <v>996</v>
+      </c>
+      <c r="D86" t="s">
+        <v>49</v>
+      </c>
+      <c r="E86" t="s">
+        <v>293</v>
+      </c>
+      <c r="F86" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>295</v>
+      </c>
+      <c r="B87" t="s">
+        <v>296</v>
+      </c>
+      <c r="C87">
+        <v>1040</v>
+      </c>
+      <c r="D87" t="s">
+        <v>49</v>
+      </c>
+      <c r="E87" t="s">
+        <v>297</v>
+      </c>
+      <c r="F87" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>298</v>
+      </c>
+      <c r="B88" t="s">
+        <v>299</v>
+      </c>
+      <c r="C88">
+        <v>33</v>
+      </c>
+      <c r="D88" t="s">
+        <v>300</v>
+      </c>
+      <c r="E88" t="s">
+        <v>301</v>
+      </c>
+      <c r="F88" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>302</v>
+      </c>
+      <c r="B89" t="s">
+        <v>303</v>
+      </c>
+      <c r="C89">
+        <v>617</v>
+      </c>
+      <c r="D89" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" t="s">
+        <v>304</v>
+      </c>
+      <c r="F89" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>305</v>
+      </c>
+      <c r="B90" t="s">
+        <v>306</v>
+      </c>
+      <c r="C90">
+        <v>40</v>
+      </c>
+      <c r="D90" t="s">
+        <v>137</v>
+      </c>
+      <c r="E90" t="s">
+        <v>307</v>
+      </c>
+      <c r="F90" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>308</v>
+      </c>
+      <c r="B91" t="s">
+        <v>309</v>
+      </c>
+      <c r="C91">
+        <v>1084</v>
+      </c>
+      <c r="D91" t="s">
+        <v>49</v>
+      </c>
+      <c r="E91" t="s">
+        <v>310</v>
+      </c>
+      <c r="F91" t="s">
         <v>284</v>
       </c>
-      <c r="B84" t="s">
-        <v>285</v>
-      </c>
-      <c r="C84">
-        <v>1179</v>
-      </c>
-      <c r="D84" t="s">
-        <v>41</v>
-      </c>
-      <c r="E84" t="s">
-        <v>286</v>
-      </c>
-      <c r="F84" t="s">
-        <v>22</v>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>311</v>
+      </c>
+      <c r="B92" t="s">
+        <v>312</v>
+      </c>
+      <c r="C92">
+        <v>1145</v>
+      </c>
+      <c r="D92" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" t="s">
+        <v>313</v>
+      </c>
+      <c r="F92" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>314</v>
+      </c>
+      <c r="B93" t="s">
+        <v>315</v>
+      </c>
+      <c r="C93">
+        <v>80</v>
+      </c>
+      <c r="D93" t="s">
+        <v>300</v>
+      </c>
+      <c r="E93" t="s">
+        <v>316</v>
+      </c>
+      <c r="F93" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F84">
-    <sortCondition descending="1" ref="F2:F84"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>